<commit_message>
changes for minimum threshold
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey_soft.xlsx
+++ b/sample_excel_files/MasterGalleryKey_soft.xlsx
@@ -520,7 +520,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -528,7 +528,16 @@
     <t xml:space="preserve">Sheetname</t>
   </si>
   <si>
+    <t xml:space="preserve">Minimum_work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedback</t>
+  </si>
+  <si>
     <t xml:space="preserve">Constant Samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need more work</t>
   </si>
   <si>
     <t xml:space="preserve">Formula Samples</t>
@@ -670,7 +679,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -692,12 +701,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -754,7 +757,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -775,17 +778,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,21 +800,39 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,7 +840,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,7 +854,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -853,36 +885,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2020</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">B2 / 10</f>
@@ -891,7 +923,7 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">ROUNDUP(B2 / 100, 0)</f>
@@ -900,7 +932,7 @@
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1000</v>
@@ -908,7 +940,7 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B6 / 1000</f>
@@ -917,26 +949,26 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B6 * 3.28084</f>
         <v>3280.84</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,7 +1002,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,10 +1010,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,10 +1032,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,10 +1051,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,10 +1062,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,10 +1073,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,10 +1084,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1082,36 +1114,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.6111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2020</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">B2 / 10</f>
@@ -1120,7 +1152,7 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">ROUNDUP(B2 / 100, 0)</f>
@@ -1129,7 +1161,7 @@
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1000</v>
@@ -1137,7 +1169,7 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B6 / 1000</f>
@@ -1146,7 +1178,7 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B6 * 3.28084</f>
@@ -1155,14 +1187,14 @@
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,7 +1205,7 @@
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">SUM(B2:B4)</f>
@@ -1182,7 +1214,7 @@
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">SUM(B2:B4) + 2</f>
@@ -1214,7 +1246,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,7 +1254,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,10 +1262,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,7 +1281,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,7 +1297,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,7 +1305,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,7 +1313,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,7 +1321,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1316,35 +1348,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2020</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">B2 / 10</f>
@@ -1353,7 +1385,7 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -1361,19 +1393,19 @@
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">ROUNDUP(B2 / 100, B4)</f>
         <v>21</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1000</v>
@@ -1381,7 +1413,7 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B7 / 1000</f>
@@ -1390,26 +1422,26 @@
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B7 * 3.28084</f>
         <v>3280.84</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B7 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,7 +1475,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,7 +1499,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1475,7 +1507,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1502,34 +1534,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2020</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">B2 / 10</f>
@@ -1538,7 +1570,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">ROUNDUP(B2 / 100, 0)</f>
@@ -1548,7 +1580,7 @@
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1000</v>
@@ -1556,7 +1588,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B6 / 1000</f>
@@ -1565,26 +1597,26 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B6 * 3.28084</f>
         <v>3280.84</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,7 +1627,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">SUM(B2:B4)</f>
@@ -1604,7 +1636,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">SUM(B2:B4) + 2</f>
@@ -1636,7 +1668,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,10 +1684,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,7 +1695,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,7 +1703,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,7 +1711,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1687,7 +1719,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,7 +1727,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,7 +1735,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,7 +1743,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>